<commit_message>
update_GDD_Review Accepting and Rejecting opened points
</commit_message>
<xml_diff>
--- a/Software Specification/Architecture/GDD/Review.xlsx
+++ b/Software Specification/Architecture/GDD/Review.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="20736" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="GDD review" sheetId="4" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="19">
   <si>
     <t>Review point</t>
   </si>
@@ -72,12 +72,21 @@
 Signal_Operator -&gt;  what do you mean about {A…D, *,#} ?
 Output from Do Math Control shall be a msg/operation result value so for msg it has no range and for result it has a range </t>
   </si>
+  <si>
+    <t>Accepted</t>
+  </si>
+  <si>
+    <t>Rejected</t>
+  </si>
+  <si>
+    <t>Do Math Control is responsible of generating the string that contains the operands, operation and result. Display Control can only accept string signals</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -465,7 +474,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -497,9 +506,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -531,6 +541,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -706,25 +717,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="59" style="9" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="47.85546875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="47.88671875" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -747,7 +758,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="60">
+    <row r="2" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
@@ -760,13 +771,15 @@
       <c r="D2" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="4"/>
+      <c r="E2" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:7" ht="30">
+    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
@@ -779,13 +792,15 @@
       <c r="D3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:7" ht="90">
+    <row r="4" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -798,13 +813,15 @@
       <c r="D4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="F4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G4" s="10"/>
     </row>
-    <row r="5" spans="1:7" ht="45">
+    <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
@@ -817,13 +834,17 @@
       <c r="D5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="4"/>
+      <c r="E5" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="F5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="10"/>
-    </row>
-    <row r="6" spans="1:7" ht="120">
+      <c r="G5" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
@@ -836,13 +857,15 @@
       <c r="D6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="F6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
@@ -855,37 +878,39 @@
       <c r="D7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="E7" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="F7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="2"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="2"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="2"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="2"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="2"/>

</xml_diff>

<commit_message>
update_GDD_Review Accepting new opened points
</commit_message>
<xml_diff>
--- a/Software Specification/Architecture/GDD/Review.xlsx
+++ b/Software Specification/Architecture/GDD/Review.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="20736" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="GDD review" sheetId="4" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="25">
   <si>
     <t>Review point</t>
   </si>
@@ -111,8 +111,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -715,7 +715,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -747,9 +747,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -781,6 +782,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -956,25 +958,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="83" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="59" style="8" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="47.85546875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="47.88671875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -997,7 +999,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="60">
+    <row r="2" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -1018,7 +1020,7 @@
       </c>
       <c r="G2" s="9"/>
     </row>
-    <row r="3" spans="1:7" ht="30">
+    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
@@ -1039,7 +1041,7 @@
       </c>
       <c r="G3" s="9"/>
     </row>
-    <row r="4" spans="1:7" ht="90">
+    <row r="4" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -1060,7 +1062,7 @@
       </c>
       <c r="G4" s="9"/>
     </row>
-    <row r="5" spans="1:7" ht="45">
+    <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -1083,7 +1085,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="120">
+    <row r="6" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
@@ -1104,7 +1106,7 @@
       </c>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
@@ -1125,7 +1127,7 @@
       </c>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="1:7" ht="90">
+    <row r="8" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>43954</v>
       </c>
@@ -1138,13 +1140,15 @@
       <c r="D8" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="F8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:7" ht="135">
+    <row r="9" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>43954</v>
       </c>
@@ -1165,7 +1169,7 @@
       </c>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:7" ht="30">
+    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>43954</v>
       </c>
@@ -1178,12 +1182,14 @@
       <c r="D10" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="3"/>
+      <c r="E10" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="F10" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="60">
+    <row r="11" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>43954</v>
       </c>
@@ -1196,12 +1202,14 @@
       <c r="D11" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="3"/>
+      <c r="E11" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="F11" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>43954</v>
       </c>

</xml_diff>

<commit_message>
update_GDD_Review updating comments (#40)
</commit_message>
<xml_diff>
--- a/Software Specification/Architecture/GDD/Review.xlsx
+++ b/Software Specification/Architecture/GDD/Review.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="27">
   <si>
     <t>Review point</t>
   </si>
@@ -106,6 +106,13 @@
   <si>
     <t>It's KEYPAD not KEYPDAD xD 
 GDD_009 &amp; GDD_010</t>
+  </si>
+  <si>
+    <t>Mali 18/3/2020: Point still open cause of point 8 is open</t>
+  </si>
+  <si>
+    <t>Mali 18/3/2020: Point still open
+Alzahraa 20/3/2020: requirement is covered in Req_PO1_DGC_GDD_002_V01 (GPIO set pin mode function)</t>
   </si>
 </sst>
 </file>
@@ -961,8 +968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="83" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="83" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1146,7 +1153,9 @@
       <c r="F8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="9"/>
+      <c r="G8" s="9" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
@@ -1186,7 +1195,7 @@
         <v>16</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -1207,6 +1216,9 @@
       </c>
       <c r="F11" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>